<commit_message>
updated to work with current inventory, oct/11/2020
</commit_message>
<xml_diff>
--- a/자동 변환기/tables/products_export_balmuda.xlsx
+++ b/자동 변환기/tables/products_export_balmuda.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mandu\OneDrive\Desktop\자동 변환기\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A1CC13-3E0B-424D-979C-AE0107689F8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95CF721F-7154-4AF3-9B5F-03B88C6083F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6045" yWindow="6915" windowWidth="24660" windowHeight="13905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3675" yWindow="1170" windowWidth="24660" windowHeight="13905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="products_export_1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="147">
   <si>
     <t>key</t>
   </si>
@@ -449,6 +449,18 @@
   </si>
   <si>
     <t>MAKR-WORK/NAVY</t>
+  </si>
+  <si>
+    <t>MAKR™ Work Carryall - TOBACCO</t>
+  </si>
+  <si>
+    <t>MAKR-WORK/TOBACCO</t>
+  </si>
+  <si>
+    <t>MAKR™ Zip Luxe Wallet - BLACK</t>
+  </si>
+  <si>
+    <t>MAKR-ZIPLUX/BLACK</t>
   </si>
 </sst>
 </file>
@@ -591,7 +603,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -771,8 +783,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor theme="9" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -887,6 +905,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -932,8 +976,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - 강조색1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1289,10 +1337,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B74"/>
+  <dimension ref="A1:B76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1494,403 +1542,419 @@
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="4" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="A27" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="2" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="4" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="A29" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="2" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="A30" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="4" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="A31" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="2" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="A32" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="4" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="A33" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="2" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="A34" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="4" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="A35" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="2" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="A36" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="4" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="A37" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="2" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="A38" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="4" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="A39" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="2" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="A40" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="4" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="A41" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="2" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="A42" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="4" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="A43" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="2" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="A44" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="4" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="A45" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="2" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="A46" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="4" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="A47" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="2" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="A48" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="4" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="A49" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="2" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="A50" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="4" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="A51" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="2" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="A52" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="4" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="A53" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="2" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+      <c r="A54" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="4" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="A55" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="2" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+      <c r="A56" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="4" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="A57" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="2" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+      <c r="A58" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="4" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+      <c r="A59" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="2" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+      <c r="A60" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="4" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+      <c r="A61" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="2" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+      <c r="A62" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="4" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+      <c r="A63" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="2" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+      <c r="A64" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="4" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+      <c r="A65" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="2" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+      <c r="A66" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="4" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+      <c r="A67" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="2" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+      <c r="A68" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="4" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+      <c r="A69" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="2" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+      <c r="A70" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="4" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+      <c r="A71" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" s="2" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+      <c r="A72" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" s="4" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+      <c r="A73" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" s="2" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+      <c r="A74" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" s="4" t="s">
         <v>142</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>